<commit_message>
Fixing bugs with parsing leagues.
</commit_message>
<xml_diff>
--- a/Parsing_assignment.xlsx
+++ b/Parsing_assignment.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_projects\BasketBallStat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1AAF2-F996-40C2-8110-EFB7E3C3F74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Parse" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="326">
   <si>
     <t>League</t>
   </si>
@@ -43,15 +37,15 @@
     <t>CBA</t>
   </si>
   <si>
-    <t>NBB</t>
-  </si>
-  <si>
     <t>Euroleague</t>
   </si>
   <si>
     <t>KBL</t>
   </si>
   <si>
+    <t>IBL</t>
+  </si>
+  <si>
     <t>Boston Celtics</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>Zhejiang-Guangsha-Lions</t>
   </si>
   <si>
-    <t>BRBBrasilia</t>
-  </si>
-  <si>
     <t>ALBA Berlin</t>
   </si>
   <si>
@@ -289,52 +280,52 @@
     <t>Wonju DB</t>
   </si>
   <si>
-    <t>Caxias do Sul Basquete</t>
-  </si>
-  <si>
-    <t>Cerrado Basquete Brasilia</t>
-  </si>
-  <si>
-    <t>Clube de Regatas do Flamengo</t>
-  </si>
-  <si>
-    <t>Esporte Clube Pinheiros Sao Paolo</t>
-  </si>
-  <si>
-    <t>Fortaleza B.C. Cearense</t>
-  </si>
-  <si>
-    <t>LuvixUniao Corinthians</t>
-  </si>
-  <si>
-    <t>Minas Belo Horizonte</t>
-  </si>
-  <si>
-    <t>Pato Basquete</t>
-  </si>
-  <si>
-    <t>PaulistanoCorpore Sao Paolo</t>
-  </si>
-  <si>
-    <t>Rio Claro Basquete</t>
-  </si>
-  <si>
-    <t>Sao Jose dos Campos</t>
-  </si>
-  <si>
-    <t>Sao Paulo FC</t>
-  </si>
-  <si>
-    <t>Sesi Franca Basquete Sao Paulo</t>
-  </si>
-  <si>
-    <t>Sport Club Corinthians Paulista</t>
-  </si>
-  <si>
-    <t>UniFacisa Paraiba</t>
-  </si>
-  <si>
-    <t>Zapone GocilBauru Basket</t>
+    <t>Amartha Hangtuah Jakarta</t>
+  </si>
+  <si>
+    <t>Bali United</t>
+  </si>
+  <si>
+    <t>Bumi Borneo Basketball Pontianak</t>
+  </si>
+  <si>
+    <t>Dewa United Surabaya</t>
+  </si>
+  <si>
+    <t>DNA Bima Perkasa Jogja</t>
+  </si>
+  <si>
+    <t>Evos Thunder Bogor</t>
+  </si>
+  <si>
+    <t>Indonesia Patriots</t>
+  </si>
+  <si>
+    <t>NSH Mountain Gold Timika</t>
+  </si>
+  <si>
+    <t>Pacific Caesar Surabaya</t>
+  </si>
+  <si>
+    <t>Pelita Jaya Bakrie Jakarta</t>
+  </si>
+  <si>
+    <t>Prawira Bandung</t>
+  </si>
+  <si>
+    <t>Rans Pik Basketball</t>
+  </si>
+  <si>
+    <t>Satria Muda Pertamina Jakarta</t>
+  </si>
+  <si>
+    <t>Satya Wacana Salatiga</t>
+  </si>
+  <si>
+    <t>Tangerang Hawks</t>
+  </si>
+  <si>
+    <t>West Bandits Solo</t>
   </si>
   <si>
     <t>Boston C</t>
@@ -946,55 +937,52 @@
     <t>https://basketball.asia-basket.com/team/South-Korea/Wonju-DB/3443?Page=2</t>
   </si>
   <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/BRB/Brasilia/6020?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Caxias-do-Sul-Basquete/12303?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Cerrado-Basquete-Brasilia/32710?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Clube-de-Regatas-do-Flamengo/1597?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Esporte-Clube-Pinheiros-Sao-Paolo/2807?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Fortaleza-BC-Cearense/17370?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Luvix/Uniao-Corinthians/1600?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Minas-Belo-Horizonte/1798?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Pato-Basquete/37007?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Paulistano/Corpore-Sao-Paolo/3557?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Rio-Claro-Basquete/14396?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Sao-Jose-dos-Campos/10293?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Sao-Paulo-FC/50954?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Sesi-Franca-Basquete-Sao-Paulo/732?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Sport-Club-Corinthians-Paulista/5926?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/UniFacisa-Paraiba/21032?Page=2</t>
-  </si>
-  <si>
-    <t>https://basketball.latinbasket.com/team/Brazil/Zapone-Gocil/Bauru-Basket/2803?Page=2</t>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Amartha-Hangtuah-Jakarta/12285?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Bali-United/62691?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Bumi-Borneo-Basketball-Pontianak/66293?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Dewa-United-Surabaya/66292?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/DNA-Bima-Perkasa-Jogja/4293?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Evos-Thunder-Bogor/66290?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Indonesia-Patriots/57359?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/NSH-Mountain-Gold-Timika/16191?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Pacific-Caesar-Surabaya/4294?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Pelita-Jaya-Bakrie-Jakarta/3245?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Prawira-Bandung/3600?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Rans-Pik-Basketball/66291?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Satria-Muda-Pertamina-Jakarta/4284?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Satya-Wacana-Salatiga/4287?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/Tangerang-Hawks/66294?Page=2</t>
+  </si>
+  <si>
+    <t>https://basketball.asia-basket.com/team/Indonesia/West-Bandits-Solo/62692?Page=2</t>
   </si>
   <si>
     <t>2020-2021</t>
@@ -1009,8 +997,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1086,14 +1074,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1140,7 +1120,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1172,27 +1152,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1224,24 +1186,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1417,23 +1361,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1458,16 +1393,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1475,16 +1410,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1492,16 +1427,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1509,16 +1444,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1526,16 +1461,16 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1543,16 +1478,16 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1560,16 +1495,16 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1577,16 +1512,16 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1594,16 +1529,16 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1614,13 +1549,13 @@
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E11" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1628,16 +1563,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1645,16 +1580,16 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E13" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1662,16 +1597,16 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E14" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1679,16 +1614,16 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E15" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1696,16 +1631,16 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1713,16 +1648,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1730,16 +1665,16 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1750,13 +1685,13 @@
         <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1764,16 +1699,16 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1781,16 +1716,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E21" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1798,16 +1733,16 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1815,16 +1750,16 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E23" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1832,16 +1767,16 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1849,16 +1784,16 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1866,16 +1801,16 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1883,16 +1818,16 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E27" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1900,16 +1835,16 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E28" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1917,16 +1852,16 @@
         <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1934,16 +1869,16 @@
         <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1951,16 +1886,16 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1968,16 +1903,16 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1985,16 +1920,16 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2002,16 +1937,16 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2019,16 +1954,16 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2036,16 +1971,16 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E36" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2053,16 +1988,16 @@
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2070,16 +2005,16 @@
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E38" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2087,16 +2022,16 @@
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E39" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -2104,16 +2039,16 @@
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E40" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2124,13 +2059,13 @@
         <v>19</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E41" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2138,16 +2073,16 @@
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E42" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2155,16 +2090,16 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E43" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2172,16 +2107,16 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E44" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2189,16 +2124,16 @@
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E45" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2206,16 +2141,16 @@
         <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E46" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2223,16 +2158,16 @@
         <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E47" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -2240,16 +2175,16 @@
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E48" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2260,13 +2195,13 @@
         <v>27</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E49" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -2274,16 +2209,16 @@
         <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -2291,16 +2226,16 @@
         <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E51" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2308,16 +2243,16 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E52" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -2325,16 +2260,16 @@
         <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E53" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -2342,16 +2277,16 @@
         <v>32</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E54" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -2359,16 +2294,16 @@
         <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E55" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -2376,16 +2311,16 @@
         <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E56" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -2393,16 +2328,16 @@
         <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E57" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -2410,16 +2345,16 @@
         <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E58" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2427,16 +2362,16 @@
         <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E59" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -2444,16 +2379,16 @@
         <v>38</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E60" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -2461,16 +2396,16 @@
         <v>39</v>
       </c>
       <c r="C61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E61" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -2478,16 +2413,16 @@
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E62" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -2495,16 +2430,16 @@
         <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E63" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -2512,16 +2447,16 @@
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E64" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -2529,16 +2464,16 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E65" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2546,16 +2481,16 @@
         <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E66" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -2563,16 +2498,16 @@
         <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E67" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -2580,16 +2515,16 @@
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E68" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -2597,16 +2532,16 @@
         <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E69" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -2614,16 +2549,16 @@
         <v>18</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E70" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2634,13 +2569,13 @@
         <v>19</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E71" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -2648,16 +2583,16 @@
         <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E72" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -2665,16 +2600,16 @@
         <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E73" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -2682,16 +2617,16 @@
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E74" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -2699,16 +2634,16 @@
         <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E75" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -2716,16 +2651,16 @@
         <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E76" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -2733,16 +2668,16 @@
         <v>25</v>
       </c>
       <c r="C77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E77" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -2750,16 +2685,16 @@
         <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E78" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -2770,13 +2705,13 @@
         <v>27</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E79" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -2784,16 +2719,16 @@
         <v>28</v>
       </c>
       <c r="C80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E80" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -2801,16 +2736,16 @@
         <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E81" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -2818,16 +2753,16 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E82" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -2835,16 +2770,16 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E83" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -2852,16 +2787,16 @@
         <v>32</v>
       </c>
       <c r="C84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E84" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -2869,16 +2804,16 @@
         <v>33</v>
       </c>
       <c r="C85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E85" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -2886,16 +2821,16 @@
         <v>34</v>
       </c>
       <c r="C86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E86" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -2903,16 +2838,16 @@
         <v>35</v>
       </c>
       <c r="C87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E87" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -2920,16 +2855,16 @@
         <v>36</v>
       </c>
       <c r="C88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E88" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -2937,16 +2872,16 @@
         <v>37</v>
       </c>
       <c r="C89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E89" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -2954,16 +2889,16 @@
         <v>38</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E90" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -2971,16 +2906,16 @@
         <v>39</v>
       </c>
       <c r="C91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E91" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2988,16 +2923,16 @@
         <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E92" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -3005,16 +2940,16 @@
         <v>41</v>
       </c>
       <c r="C93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E93" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3022,16 +2957,16 @@
         <v>42</v>
       </c>
       <c r="C94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E94" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -3039,16 +2974,16 @@
         <v>43</v>
       </c>
       <c r="C95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E95" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -3056,16 +2991,16 @@
         <v>44</v>
       </c>
       <c r="C96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E96" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -3073,16 +3008,16 @@
         <v>45</v>
       </c>
       <c r="C97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E97" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -3090,16 +3025,16 @@
         <v>46</v>
       </c>
       <c r="C98" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E98" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -3107,16 +3042,16 @@
         <v>47</v>
       </c>
       <c r="C99" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E99" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3124,16 +3059,16 @@
         <v>48</v>
       </c>
       <c r="C100" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E100" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3141,16 +3076,16 @@
         <v>49</v>
       </c>
       <c r="C101" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E101" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3158,16 +3093,16 @@
         <v>50</v>
       </c>
       <c r="C102" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E102" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3175,16 +3110,16 @@
         <v>51</v>
       </c>
       <c r="C103" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E103" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3192,16 +3127,16 @@
         <v>52</v>
       </c>
       <c r="C104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E104" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3209,16 +3144,16 @@
         <v>53</v>
       </c>
       <c r="C105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E105" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3226,16 +3161,16 @@
         <v>54</v>
       </c>
       <c r="C106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E106" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3243,16 +3178,16 @@
         <v>55</v>
       </c>
       <c r="C107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E107" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3260,16 +3195,16 @@
         <v>56</v>
       </c>
       <c r="C108" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E108" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3277,16 +3212,16 @@
         <v>57</v>
       </c>
       <c r="C109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E109" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3294,16 +3229,16 @@
         <v>58</v>
       </c>
       <c r="C110" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E110" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3311,511 +3246,511 @@
         <v>59</v>
       </c>
       <c r="C111" t="s">
+        <v>151</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E111" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" t="s">
+        <v>60</v>
+      </c>
+      <c r="C112" t="s">
         <v>152</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E111" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="E112" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113" t="s">
+        <v>61</v>
+      </c>
+      <c r="C113" t="s">
+        <v>153</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E113" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" t="s">
+        <v>62</v>
+      </c>
+      <c r="C114" t="s">
+        <v>154</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E114" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" t="s">
+        <v>155</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E115" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" t="s">
+        <v>156</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E116" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>65</v>
+      </c>
+      <c r="C117" t="s">
+        <v>157</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E117" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>66</v>
+      </c>
+      <c r="C118" t="s">
+        <v>158</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E118" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>67</v>
+      </c>
+      <c r="C119" t="s">
+        <v>159</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E119" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" t="s">
+        <v>160</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E120" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>69</v>
+      </c>
+      <c r="C121" t="s">
+        <v>161</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E121" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" t="s">
+        <v>70</v>
+      </c>
+      <c r="C122" t="s">
+        <v>162</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E122" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" t="s">
+        <v>71</v>
+      </c>
+      <c r="C123" t="s">
+        <v>163</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E123" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" t="s">
+        <v>72</v>
+      </c>
+      <c r="C124" t="s">
+        <v>164</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E124" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E125" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" t="s">
+        <v>74</v>
+      </c>
+      <c r="C126" t="s">
+        <v>74</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E126" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" t="s">
+        <v>75</v>
+      </c>
+      <c r="C127" t="s">
+        <v>166</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E127" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" t="s">
+        <v>76</v>
+      </c>
+      <c r="C128" t="s">
+        <v>167</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E128" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" t="s">
+        <v>77</v>
+      </c>
+      <c r="C129" t="s">
+        <v>168</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E129" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
         <v>8</v>
       </c>
-      <c r="B112" t="s">
-        <v>61</v>
-      </c>
-      <c r="C112" t="s">
-        <v>153</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E112" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="B130" t="s">
+        <v>78</v>
+      </c>
+      <c r="C130" t="s">
+        <v>78</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E130" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
         <v>8</v>
       </c>
-      <c r="B113" t="s">
-        <v>62</v>
-      </c>
-      <c r="C113" t="s">
-        <v>154</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E113" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="B131" t="s">
+        <v>79</v>
+      </c>
+      <c r="C131" t="s">
+        <v>79</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E131" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
         <v>8</v>
       </c>
-      <c r="B114" t="s">
-        <v>63</v>
-      </c>
-      <c r="C114" t="s">
-        <v>155</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E114" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="B132" t="s">
+        <v>80</v>
+      </c>
+      <c r="C132" t="s">
+        <v>80</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E132" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
         <v>8</v>
       </c>
-      <c r="B115" t="s">
-        <v>64</v>
-      </c>
-      <c r="C115" t="s">
-        <v>156</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E115" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="B133" t="s">
+        <v>81</v>
+      </c>
+      <c r="C133" t="s">
+        <v>81</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E133" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
         <v>8</v>
       </c>
-      <c r="B116" t="s">
-        <v>65</v>
-      </c>
-      <c r="C116" t="s">
-        <v>157</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E116" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="B134" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134" t="s">
+        <v>82</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E134" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
         <v>8</v>
       </c>
-      <c r="B117" t="s">
-        <v>66</v>
-      </c>
-      <c r="C117" t="s">
-        <v>158</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="E117" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B135" t="s">
+        <v>83</v>
+      </c>
+      <c r="C135" t="s">
+        <v>83</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E135" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
         <v>8</v>
       </c>
-      <c r="B118" t="s">
-        <v>67</v>
-      </c>
-      <c r="C118" t="s">
-        <v>159</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E118" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="B136" t="s">
+        <v>84</v>
+      </c>
+      <c r="C136" t="s">
+        <v>84</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E136" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
         <v>8</v>
       </c>
-      <c r="B119" t="s">
-        <v>68</v>
-      </c>
-      <c r="C119" t="s">
-        <v>160</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E119" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="B137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C137" t="s">
+        <v>85</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E137" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
         <v>8</v>
       </c>
-      <c r="B120" t="s">
-        <v>69</v>
-      </c>
-      <c r="C120" t="s">
-        <v>161</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E120" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="B138" t="s">
+        <v>86</v>
+      </c>
+      <c r="C138" t="s">
+        <v>86</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E138" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
         <v>8</v>
       </c>
-      <c r="B121" t="s">
-        <v>70</v>
-      </c>
-      <c r="C121" t="s">
-        <v>162</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E121" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>8</v>
-      </c>
-      <c r="B122" t="s">
-        <v>71</v>
-      </c>
-      <c r="C122" t="s">
-        <v>163</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E122" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>8</v>
-      </c>
-      <c r="B123" t="s">
-        <v>72</v>
-      </c>
-      <c r="C123" t="s">
-        <v>164</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E123" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>8</v>
-      </c>
-      <c r="B124" t="s">
-        <v>73</v>
-      </c>
-      <c r="C124" t="s">
-        <v>165</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E124" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>8</v>
-      </c>
-      <c r="B125" t="s">
-        <v>74</v>
-      </c>
-      <c r="C125" t="s">
-        <v>166</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E125" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>8</v>
-      </c>
-      <c r="B126" t="s">
-        <v>75</v>
-      </c>
-      <c r="C126" t="s">
-        <v>75</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E126" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>8</v>
-      </c>
-      <c r="B127" t="s">
-        <v>76</v>
-      </c>
-      <c r="C127" t="s">
-        <v>167</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E127" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>8</v>
-      </c>
-      <c r="B128" t="s">
-        <v>77</v>
-      </c>
-      <c r="C128" t="s">
-        <v>168</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E128" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>8</v>
-      </c>
-      <c r="B129" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" t="s">
-        <v>169</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E129" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="B139" t="s">
+        <v>87</v>
+      </c>
+      <c r="C139" t="s">
+        <v>87</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E139" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
         <v>9</v>
       </c>
-      <c r="B130" t="s">
-        <v>79</v>
-      </c>
-      <c r="C130" t="s">
-        <v>79</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E130" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B140" t="s">
+        <v>88</v>
+      </c>
+      <c r="C140" t="s">
+        <v>88</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E140" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
         <v>9</v>
-      </c>
-      <c r="B131" t="s">
-        <v>80</v>
-      </c>
-      <c r="C131" t="s">
-        <v>80</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E131" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>9</v>
-      </c>
-      <c r="B132" t="s">
-        <v>81</v>
-      </c>
-      <c r="C132" t="s">
-        <v>81</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E132" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>9</v>
-      </c>
-      <c r="B133" t="s">
-        <v>82</v>
-      </c>
-      <c r="C133" t="s">
-        <v>82</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E133" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>9</v>
-      </c>
-      <c r="B134" t="s">
-        <v>83</v>
-      </c>
-      <c r="C134" t="s">
-        <v>83</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E134" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>9</v>
-      </c>
-      <c r="B135" t="s">
-        <v>84</v>
-      </c>
-      <c r="C135" t="s">
-        <v>84</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E135" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>9</v>
-      </c>
-      <c r="B136" t="s">
-        <v>85</v>
-      </c>
-      <c r="C136" t="s">
-        <v>85</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E136" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>9</v>
-      </c>
-      <c r="B137" t="s">
-        <v>86</v>
-      </c>
-      <c r="C137" t="s">
-        <v>86</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E137" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>9</v>
-      </c>
-      <c r="B138" t="s">
-        <v>87</v>
-      </c>
-      <c r="C138" t="s">
-        <v>87</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E138" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>9</v>
-      </c>
-      <c r="B139" t="s">
-        <v>88</v>
-      </c>
-      <c r="C139" t="s">
-        <v>88</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E139" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>7</v>
-      </c>
-      <c r="B140" t="s">
-        <v>60</v>
-      </c>
-      <c r="C140" t="s">
-        <v>60</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E140" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>7</v>
       </c>
       <c r="B141" t="s">
         <v>89</v>
@@ -3824,15 +3759,15 @@
         <v>89</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E141" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B142" t="s">
         <v>90</v>
@@ -3841,15 +3776,15 @@
         <v>90</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E142" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B143" t="s">
         <v>91</v>
@@ -3858,15 +3793,15 @@
         <v>91</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E143" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B144" t="s">
         <v>92</v>
@@ -3875,15 +3810,15 @@
         <v>92</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E144" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
         <v>93</v>
@@ -3892,15 +3827,15 @@
         <v>93</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E145" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B146" t="s">
         <v>94</v>
@@ -3909,15 +3844,15 @@
         <v>94</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E146" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B147" t="s">
         <v>95</v>
@@ -3926,15 +3861,15 @@
         <v>95</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E147" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B148" t="s">
         <v>96</v>
@@ -3943,15 +3878,15 @@
         <v>96</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E148" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B149" t="s">
         <v>97</v>
@@ -3960,15 +3895,15 @@
         <v>97</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E149" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B150" t="s">
         <v>98</v>
@@ -3977,15 +3912,15 @@
         <v>98</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E150" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B151" t="s">
         <v>99</v>
@@ -3994,15 +3929,15 @@
         <v>99</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E151" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B152" t="s">
         <v>100</v>
@@ -4011,15 +3946,15 @@
         <v>100</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E152" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B153" t="s">
         <v>101</v>
@@ -4028,15 +3963,15 @@
         <v>101</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E153" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B154" t="s">
         <v>102</v>
@@ -4045,15 +3980,15 @@
         <v>102</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E154" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B155" t="s">
         <v>103</v>
@@ -4062,186 +3997,168 @@
         <v>103</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E155" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>7</v>
-      </c>
-      <c r="B156" t="s">
-        <v>104</v>
-      </c>
-      <c r="C156" t="s">
-        <v>104</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E156" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="D41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="D52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="D53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="D58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="D61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="D62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="D64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="D65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="D69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="D72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="D80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="D83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="D84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="D86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="D87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="D90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="D91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="D92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="D98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="D100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="D101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="D103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="D104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="D105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="D107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="D109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="D110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="D111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="D113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="D114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="D115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="D116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="D117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="D118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="D119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="D120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="D121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="D122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="D123" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="D124" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="D125" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="D126" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="D127" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="D128" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="D129" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="D130" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="D131" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="D132" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="D133" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="D134" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="D135" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="D136" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="D137" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="D138" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="D139" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="D140" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="D141" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="D142" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="D143" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="D144" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="D145" r:id="rId144" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="D146" r:id="rId145" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="D147" r:id="rId146" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="D148" r:id="rId147" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="D149" r:id="rId148" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="D150" r:id="rId149" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="D151" r:id="rId150" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="D152" r:id="rId151" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="D153" r:id="rId152" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="D154" r:id="rId153" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="D155" r:id="rId154" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="D156" r:id="rId155" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
+    <hyperlink ref="D84" r:id="rId83"/>
+    <hyperlink ref="D85" r:id="rId84"/>
+    <hyperlink ref="D86" r:id="rId85"/>
+    <hyperlink ref="D87" r:id="rId86"/>
+    <hyperlink ref="D88" r:id="rId87"/>
+    <hyperlink ref="D89" r:id="rId88"/>
+    <hyperlink ref="D90" r:id="rId89"/>
+    <hyperlink ref="D91" r:id="rId90"/>
+    <hyperlink ref="D92" r:id="rId91"/>
+    <hyperlink ref="D93" r:id="rId92"/>
+    <hyperlink ref="D94" r:id="rId93"/>
+    <hyperlink ref="D95" r:id="rId94"/>
+    <hyperlink ref="D96" r:id="rId95"/>
+    <hyperlink ref="D97" r:id="rId96"/>
+    <hyperlink ref="D98" r:id="rId97"/>
+    <hyperlink ref="D99" r:id="rId98"/>
+    <hyperlink ref="D100" r:id="rId99"/>
+    <hyperlink ref="D101" r:id="rId100"/>
+    <hyperlink ref="D102" r:id="rId101"/>
+    <hyperlink ref="D103" r:id="rId102"/>
+    <hyperlink ref="D104" r:id="rId103"/>
+    <hyperlink ref="D105" r:id="rId104"/>
+    <hyperlink ref="D106" r:id="rId105"/>
+    <hyperlink ref="D107" r:id="rId106"/>
+    <hyperlink ref="D108" r:id="rId107"/>
+    <hyperlink ref="D109" r:id="rId108"/>
+    <hyperlink ref="D110" r:id="rId109"/>
+    <hyperlink ref="D111" r:id="rId110"/>
+    <hyperlink ref="D112" r:id="rId111"/>
+    <hyperlink ref="D113" r:id="rId112"/>
+    <hyperlink ref="D114" r:id="rId113"/>
+    <hyperlink ref="D115" r:id="rId114"/>
+    <hyperlink ref="D116" r:id="rId115"/>
+    <hyperlink ref="D117" r:id="rId116"/>
+    <hyperlink ref="D118" r:id="rId117"/>
+    <hyperlink ref="D119" r:id="rId118"/>
+    <hyperlink ref="D120" r:id="rId119"/>
+    <hyperlink ref="D121" r:id="rId120"/>
+    <hyperlink ref="D122" r:id="rId121"/>
+    <hyperlink ref="D123" r:id="rId122"/>
+    <hyperlink ref="D124" r:id="rId123"/>
+    <hyperlink ref="D125" r:id="rId124"/>
+    <hyperlink ref="D126" r:id="rId125"/>
+    <hyperlink ref="D127" r:id="rId126"/>
+    <hyperlink ref="D128" r:id="rId127"/>
+    <hyperlink ref="D129" r:id="rId128"/>
+    <hyperlink ref="D130" r:id="rId129"/>
+    <hyperlink ref="D131" r:id="rId130"/>
+    <hyperlink ref="D132" r:id="rId131"/>
+    <hyperlink ref="D133" r:id="rId132"/>
+    <hyperlink ref="D134" r:id="rId133"/>
+    <hyperlink ref="D135" r:id="rId134"/>
+    <hyperlink ref="D136" r:id="rId135"/>
+    <hyperlink ref="D137" r:id="rId136"/>
+    <hyperlink ref="D138" r:id="rId137"/>
+    <hyperlink ref="D139" r:id="rId138"/>
+    <hyperlink ref="D140" r:id="rId139"/>
+    <hyperlink ref="D141" r:id="rId140"/>
+    <hyperlink ref="D142" r:id="rId141"/>
+    <hyperlink ref="D143" r:id="rId142"/>
+    <hyperlink ref="D144" r:id="rId143"/>
+    <hyperlink ref="D145" r:id="rId144"/>
+    <hyperlink ref="D146" r:id="rId145"/>
+    <hyperlink ref="D147" r:id="rId146"/>
+    <hyperlink ref="D148" r:id="rId147"/>
+    <hyperlink ref="D149" r:id="rId148"/>
+    <hyperlink ref="D150" r:id="rId149"/>
+    <hyperlink ref="D151" r:id="rId150"/>
+    <hyperlink ref="D152" r:id="rId151"/>
+    <hyperlink ref="D153" r:id="rId152"/>
+    <hyperlink ref="D154" r:id="rId153"/>
+    <hyperlink ref="D155" r:id="rId154"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>